<commit_message>
added more drugs to database, with different is_active values updated logic.py to reflect functionality of excel logic version
</commit_message>
<xml_diff>
--- a/PT_portfolio/source/DrugDescriptions.xlsx
+++ b/PT_portfolio/source/DrugDescriptions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>RANK</t>
   </si>
@@ -102,12 +102,48 @@
   <si>
     <t>38543111000001106</t>
   </si>
+  <si>
+    <t>Metformin 1g modified-release tablets (Brown &amp; Burk UK Ltd)</t>
+  </si>
+  <si>
+    <t>42241011000001108</t>
+  </si>
+  <si>
+    <t>Omeprazole 20mg gastro-resistant tablets (Dexcel-Pharma Ltd)</t>
+  </si>
+  <si>
+    <t>11552111000001108</t>
+  </si>
+  <si>
+    <t>Atorvastatin 20mg tablets (Teva UK Ltd)</t>
+  </si>
+  <si>
+    <t>20494411000001102</t>
+  </si>
+  <si>
+    <t>Ramipril 2.5mg capsules (Crescent Pharma Ltd)</t>
+  </si>
+  <si>
+    <t>38578211000001109</t>
+  </si>
+  <si>
+    <t>white-orange</t>
+  </si>
+  <si>
+    <t>Ramipril 5mg capsules (Crescent Pharma Ltd)</t>
+  </si>
+  <si>
+    <t>38739511000001103</t>
+  </si>
+  <si>
+    <t>white-green</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -126,8 +162,12 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF212B32"/>
+      <name val="&quot;Frutiger W01&quot;"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +186,12 @@
         <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F4F5"/>
+        <bgColor rgb="FFF0F4F5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -153,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -167,6 +213,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -429,8 +478,8 @@
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="b">
-        <v>1</v>
+      <c r="D2" s="3">
+        <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>10</v>
@@ -455,8 +504,8 @@
       <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="b">
-        <v>1</v>
+      <c r="D3" s="3">
+        <v>1.0</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
@@ -479,8 +528,8 @@
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="b">
-        <v>1</v>
+      <c r="D4" s="3">
+        <v>1.0</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>10</v>
@@ -505,8 +554,8 @@
       <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="b">
-        <v>1</v>
+      <c r="D5" s="3">
+        <v>1.0</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>10</v>
@@ -531,8 +580,8 @@
       <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3" t="b">
-        <v>1</v>
+      <c r="D6" s="3">
+        <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>10</v>
@@ -557,8 +606,8 @@
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="3" t="b">
-        <v>1</v>
+      <c r="D7" s="3">
+        <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>10</v>
@@ -574,57 +623,131 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="A8" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="A10" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="4"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -634,7 +757,7 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="4"/>
+      <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>

</xml_diff>